<commit_message>
adworks dw fixing file names
</commit_message>
<xml_diff>
--- a/ad_works_dw/pipelines/tables.xlsx
+++ b/ad_works_dw/pipelines/tables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works_dw/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034619C6-15D4-B644-A145-6B28AE071F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394535C8-DD86-F749-BE25-CCC138C36F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="1240" windowWidth="29580" windowHeight="21100" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$32:$G$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$31:$G$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="141">
   <si>
     <t>stage</t>
   </si>
@@ -137,172 +137,7 @@
     <t>landing_ad_works_dw</t>
   </si>
   <si>
-    <t>dbo_dim_account</t>
-  </si>
-  <si>
-    <t>dbo_dim_currency</t>
-  </si>
-  <si>
-    <t>dbo_dim_customer</t>
-  </si>
-  <si>
-    <t>dbo_dim_date</t>
-  </si>
-  <si>
-    <t>dbo_dim_department_group</t>
-  </si>
-  <si>
-    <t>dbo_dim_employee</t>
-  </si>
-  <si>
-    <t>dbo_dim_geography</t>
-  </si>
-  <si>
-    <t>dbo_dim_organization</t>
-  </si>
-  <si>
-    <t>dbo_dim_product</t>
-  </si>
-  <si>
-    <t>dbo_dim_product_category</t>
-  </si>
-  <si>
-    <t>dbo_dim_product_subcategory</t>
-  </si>
-  <si>
-    <t>dbo_dim_promotion</t>
-  </si>
-  <si>
-    <t>dbo_dim_eseller</t>
-  </si>
-  <si>
-    <t>dbo_dim_salesreason</t>
-  </si>
-  <si>
-    <t>dbo_dim_salesterritory</t>
-  </si>
-  <si>
-    <t>dbo_dim_scenario</t>
-  </si>
-  <si>
-    <t>dbo_fact_additional_international_product_description</t>
-  </si>
-  <si>
-    <t>dbo_fact_call_center</t>
-  </si>
-  <si>
-    <t>dbo_fact_currency_rate</t>
-  </si>
-  <si>
-    <t>dbo_fact_finance</t>
-  </si>
-  <si>
-    <t>dbo_fact_internet_sales</t>
-  </si>
-  <si>
-    <t>dbo_fact_internet_sales_reason</t>
-  </si>
-  <si>
-    <t>dbo_fact_product_inventory</t>
-  </si>
-  <si>
-    <t>dbo_fact_reseller_sales</t>
-  </si>
-  <si>
-    <t>dbo_fact_sales_quota</t>
-  </si>
-  <si>
-    <t>dbo_fact_survey_response</t>
-  </si>
-  <si>
-    <t>dbo_new_fact_currency_rate</t>
-  </si>
-  <si>
-    <t>dbo_prospective_buyer</t>
-  </si>
-  <si>
     <t>raw_ad_works_dw</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_account</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_currency</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_customer</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_date</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_department_group</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_employee</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_geography</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_organization</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_product</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_product_category</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_product_subcategory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_promotion</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_eseller</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_salesreason</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_salesterritory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_dim_scenario</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_additional_international_product_description</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_call_center</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_currency_rate</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_finance</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_internet_sales</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_internet_sales_reason</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_product_inventory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_reseller_sales</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_sales_quota</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_fact_survey_response</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works_dw.dbo_prospective_buyer</t>
   </si>
   <si>
     <t>AccountKey</t>
@@ -472,6 +307,168 @@
   </si>
   <si>
     <t>raw.raw_ad_works_dw.*</t>
+  </si>
+  <si>
+    <t>dbo_DimAccount</t>
+  </si>
+  <si>
+    <t>dbo_DimCurrency</t>
+  </si>
+  <si>
+    <t>dbo_DimCustomer</t>
+  </si>
+  <si>
+    <t>dbo_DimDate</t>
+  </si>
+  <si>
+    <t>dbo_DimDepartmentGroup</t>
+  </si>
+  <si>
+    <t>dbo_DimEmployee</t>
+  </si>
+  <si>
+    <t>dbo_DimGeography</t>
+  </si>
+  <si>
+    <t>dbo_DimOrganization</t>
+  </si>
+  <si>
+    <t>dbo_DimProduct</t>
+  </si>
+  <si>
+    <t>dbo_DimProductCategory</t>
+  </si>
+  <si>
+    <t>dbo_DimProductSubcategory</t>
+  </si>
+  <si>
+    <t>dbo_DimPromotion</t>
+  </si>
+  <si>
+    <t>dbo_DimReseller</t>
+  </si>
+  <si>
+    <t>dbo_DimSalesReason</t>
+  </si>
+  <si>
+    <t>dbo_SimSalesTerritory</t>
+  </si>
+  <si>
+    <t>dbo_DimScenario</t>
+  </si>
+  <si>
+    <t>dbo_FactAdditionalInternationalProductDescription</t>
+  </si>
+  <si>
+    <t>dbo_factCallCenter</t>
+  </si>
+  <si>
+    <t>dbo_FactCurrencyRate</t>
+  </si>
+  <si>
+    <t>dbo_FactFinance</t>
+  </si>
+  <si>
+    <t>dbo_FactInternetSales</t>
+  </si>
+  <si>
+    <t>dbo_FactInternetSalesReason</t>
+  </si>
+  <si>
+    <t>dbo_FactProductInventory</t>
+  </si>
+  <si>
+    <t>dbo_FactResellerSales</t>
+  </si>
+  <si>
+    <t>dbo_FactSalesQuota</t>
+  </si>
+  <si>
+    <t>dbo_FactSurveyResponse</t>
+  </si>
+  <si>
+    <t>dbo_ProspectiveBuyer</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimAccount</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimCurrency</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimCustomer</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimDate</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimDepartmentGroup</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimEmployee</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimGeography</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimOrganization</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimProduct</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimProductCategory</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimProductSubcategory</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimPromotion</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimReseller</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimSalesReason</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_SimSalesTerritory</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_DimScenario</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactAdditionalInternationalProductDescription</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_factCallCenter</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactCurrencyRate</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactFinance</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactInternetSales</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactInternetSalesReason</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactProductInventory</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactResellerSales</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactSalesQuota</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_FactSurveyResponse</t>
+  </si>
+  <si>
+    <t>landing.landing_ad_works_dw.dbo_ProspectiveBuyer</t>
   </si>
 </sst>
 </file>
@@ -628,16 +625,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -959,11 +956,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,25 +993,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="24" t="s">
@@ -1025,31 +1022,31 @@
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="22" t="s">
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
       <c r="V1" s="25" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:24" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -1117,7 +1114,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1150,7 +1147,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1164,7 +1161,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1178,7 +1175,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1192,7 +1189,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1206,7 +1203,7 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1220,7 +1217,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1234,7 +1231,7 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1248,7 +1245,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1262,7 +1259,7 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1276,7 +1273,7 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1290,7 +1287,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1304,7 +1301,7 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1318,7 +1315,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1332,7 +1329,7 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1346,7 +1343,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1360,7 +1357,7 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1374,7 +1371,7 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1388,7 +1385,7 @@
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1402,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1416,7 +1413,7 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1430,7 +1427,7 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1444,7 +1441,7 @@
         <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1458,7 +1455,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1472,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1486,7 +1483,7 @@
         <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1500,7 +1497,7 @@
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -1514,22 +1511,46 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
       </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="6">
+        <v>30</v>
+      </c>
+      <c r="S31" s="2">
+        <v>0</v>
+      </c>
+      <c r="U31" s="2">
+        <v>1</v>
+      </c>
+      <c r="V31" s="18">
+        <v>1</v>
+      </c>
+      <c r="W31" s="16">
+        <v>365</v>
+      </c>
     </row>
     <row r="32" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -1539,16 +1560,16 @@
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
         <v>60</v>
       </c>
-      <c r="D32" t="s">
-        <v>114</v>
-      </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>25</v>
@@ -1577,16 +1598,16 @@
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>25</v>
@@ -1615,16 +1636,16 @@
         <v>14</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>25</v>
@@ -1653,16 +1674,16 @@
         <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>25</v>
@@ -1691,16 +1712,16 @@
         <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>25</v>
@@ -1729,16 +1750,16 @@
         <v>14</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>25</v>
@@ -1767,16 +1788,16 @@
         <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>25</v>
@@ -1805,16 +1826,16 @@
         <v>14</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>25</v>
@@ -1843,16 +1864,16 @@
         <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>25</v>
@@ -1881,16 +1902,16 @@
         <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>123</v>
+        <v>69</v>
       </c>
       <c r="F41" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>25</v>
@@ -1919,16 +1940,16 @@
         <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>25</v>
@@ -1957,16 +1978,16 @@
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>25</v>
@@ -1995,16 +2016,16 @@
         <v>14</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>25</v>
@@ -2033,16 +2054,16 @@
         <v>14</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>25</v>
@@ -2071,16 +2092,16 @@
         <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>25</v>
@@ -2109,244 +2130,244 @@
         <v>14</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="F47" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="6">
+        <v>30</v>
+      </c>
+      <c r="S47" s="2">
+        <v>0</v>
+      </c>
+      <c r="U47" s="2">
+        <v>1</v>
+      </c>
+      <c r="V47" s="18">
+        <v>1</v>
+      </c>
+      <c r="W47" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
         <v>76</v>
       </c>
-      <c r="L47" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="6">
-        <v>30</v>
-      </c>
-      <c r="S47" s="2">
-        <v>0</v>
-      </c>
-      <c r="U47" s="2">
-        <v>1</v>
-      </c>
-      <c r="V47" s="18">
-        <v>1</v>
-      </c>
-      <c r="W47" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" t="s">
-        <v>130</v>
-      </c>
-      <c r="F48" t="s">
-        <v>96</v>
+      <c r="F48" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="6">
+        <v>30</v>
+      </c>
+      <c r="S48" s="2">
+        <v>0</v>
+      </c>
+      <c r="U48" s="2">
+        <v>1</v>
+      </c>
+      <c r="V48" s="18">
+        <v>1</v>
+      </c>
+      <c r="W48" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="6">
-        <v>30</v>
-      </c>
-      <c r="S48" s="2">
-        <v>0</v>
-      </c>
-      <c r="U48" s="2">
-        <v>1</v>
-      </c>
-      <c r="V48" s="18">
-        <v>1</v>
-      </c>
-      <c r="W48" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" t="s">
-        <v>131</v>
-      </c>
       <c r="F49" s="19" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="6">
+        <v>30</v>
+      </c>
+      <c r="S49" s="2">
+        <v>0</v>
+      </c>
+      <c r="U49" s="2">
+        <v>1</v>
+      </c>
+      <c r="V49" s="18">
+        <v>1</v>
+      </c>
+      <c r="W49" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s">
         <v>78</v>
       </c>
-      <c r="L49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M49" s="6">
-        <v>30</v>
-      </c>
-      <c r="S49" s="2">
-        <v>0</v>
-      </c>
-      <c r="U49" s="2">
-        <v>1</v>
-      </c>
-      <c r="V49" s="18">
-        <v>1</v>
-      </c>
-      <c r="W49" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="19" t="s">
-        <v>104</v>
+      <c r="F50" t="s">
+        <v>50</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="6">
+        <v>30</v>
+      </c>
+      <c r="S50" s="2">
+        <v>0</v>
+      </c>
+      <c r="U50" s="2">
+        <v>1</v>
+      </c>
+      <c r="V50" s="18">
+        <v>1</v>
+      </c>
+      <c r="W50" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s">
         <v>79</v>
       </c>
-      <c r="L50" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M50" s="6">
-        <v>30</v>
-      </c>
-      <c r="S50" s="2">
-        <v>0</v>
-      </c>
-      <c r="U50" s="2">
-        <v>1</v>
-      </c>
-      <c r="V50" s="18">
-        <v>1</v>
-      </c>
-      <c r="W50" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" t="s">
-        <v>105</v>
+      <c r="F51" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="6">
+        <v>30</v>
+      </c>
+      <c r="S51" s="2">
+        <v>0</v>
+      </c>
+      <c r="U51" s="2">
+        <v>1</v>
+      </c>
+      <c r="V51" s="18">
+        <v>1</v>
+      </c>
+      <c r="W51" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" t="s">
         <v>80</v>
       </c>
-      <c r="L51" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M51" s="6">
-        <v>30</v>
-      </c>
-      <c r="S51" s="2">
-        <v>0</v>
-      </c>
-      <c r="U51" s="2">
-        <v>1</v>
-      </c>
-      <c r="V51" s="18">
-        <v>1</v>
-      </c>
-      <c r="W51" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" t="s">
-        <v>134</v>
-      </c>
       <c r="F52" s="19" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="6">
+        <v>30</v>
+      </c>
+      <c r="S52" s="2">
+        <v>0</v>
+      </c>
+      <c r="U52" s="2">
+        <v>1</v>
+      </c>
+      <c r="V52" s="18">
+        <v>1</v>
+      </c>
+      <c r="W52" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
         <v>81</v>
       </c>
-      <c r="L52" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M52" s="6">
-        <v>30</v>
-      </c>
-      <c r="S52" s="2">
-        <v>0</v>
-      </c>
-      <c r="U52" s="2">
-        <v>1</v>
-      </c>
-      <c r="V52" s="18">
-        <v>1</v>
-      </c>
-      <c r="W52" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" t="s">
-        <v>135</v>
-      </c>
       <c r="F53" s="19" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>25</v>
@@ -2375,54 +2396,54 @@
         <v>14</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>108</v>
+        <v>82</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" s="6">
+        <v>30</v>
+      </c>
+      <c r="S54" s="2">
+        <v>0</v>
+      </c>
+      <c r="U54" s="2">
+        <v>1</v>
+      </c>
+      <c r="V54" s="18">
+        <v>1</v>
+      </c>
+      <c r="W54" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s">
         <v>83</v>
       </c>
-      <c r="L54" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M54" s="6">
-        <v>30</v>
-      </c>
-      <c r="S54" s="2">
-        <v>0</v>
-      </c>
-      <c r="U54" s="2">
-        <v>1</v>
-      </c>
-      <c r="V54" s="18">
-        <v>1</v>
-      </c>
-      <c r="W54" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" t="s">
-        <v>137</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>106</v>
+      <c r="F55" t="s">
+        <v>54</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>25</v>
@@ -2451,16 +2472,16 @@
         <v>14</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="F56" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>25</v>
@@ -2489,16 +2510,16 @@
         <v>14</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>25</v>
@@ -2519,83 +2540,45 @@
         <v>365</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" t="s">
-        <v>140</v>
-      </c>
-      <c r="F58" t="s">
-        <v>111</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M58" s="6">
-        <v>30</v>
-      </c>
-      <c r="S58" s="2">
-        <v>0</v>
-      </c>
-      <c r="U58" s="2">
-        <v>1</v>
-      </c>
-      <c r="V58" s="18">
-        <v>1</v>
-      </c>
-      <c r="W58" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="6"/>
-      <c r="N60" s="6"/>
-      <c r="O60" s="6"/>
-      <c r="P60" s="6"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="6"/>
-      <c r="S60" s="6"/>
-      <c r="T60" s="6"/>
-      <c r="U60" s="6"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="17"/>
-      <c r="X60" s="6"/>
+    <row r="59" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="17"/>
+      <c r="X59" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>